<commit_message>
rename coordinate attributes for visual census spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheets_final/marinegeo_spreadsheet_seagrass_shoots.xlsx
+++ b/spreadsheets_final/marinegeo_spreadsheet_seagrass_shoots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\spreadsheets_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579F7C35-1653-4DBC-AD6F-EC0AF0048E05}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B799C19B-C7CC-40F0-8977-B0E048BE9BC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="2040" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -2584,7 +2584,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="50.1" customHeight="1"/>

</xml_diff>